<commit_message>
1. Implementing adaptive execution (sequential) 2. Implementing several stability-criteria as helper functions and a functionality for a manual user input „custom_stability_function“ 3. Adjusting the meta-level with specific response if engine-type is „execution_adaptive_“ 4. Implementing new splitter-engine: split_random_stratified
</commit_message>
<xml_diff>
--- a/tests/publish_exports/excel_basis_test_singleelement.xlsx
+++ b/tests/publish_exports/excel_basis_test_singleelement.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">split</t>
   </si>
@@ -71,22 +71,19 @@
     <t xml:space="preserve">summarystats_range</t>
   </si>
   <si>
-    <t xml:space="preserve">fold1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fold2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fold3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fold4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fold5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fold6</t>
+    <t xml:space="preserve">split1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">split2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">split3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">split4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">split5</t>
   </si>
 </sst>
 </file>
@@ -482,58 +479,58 @@
         <v>19</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0843109446082154</v>
+        <v>0.105465445923025</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0168634912571232</v>
+        <v>0.00968446487245028</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0168634912571232</v>
+        <v>0.00968446487245028</v>
       </c>
       <c r="E2" t="n">
-        <v>0.012616509696345</v>
+        <v>0.0101702486418485</v>
       </c>
       <c r="F2" t="n">
-        <v>0.000245643380238053</v>
+        <v>0.00690566616132421</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00855401391080068</v>
+        <v>0.0137561491366818</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0903614457831325</v>
+        <v>0.12</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0879714748774965</v>
+        <v>0.117599928568928</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0319658089736956</v>
+        <v>0.0284239643932029</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0010218129433428</v>
+        <v>0.000807921751826065</v>
       </c>
       <c r="L2" t="n">
-        <v>0.020536916522099</v>
+        <v>0.049221387125471</v>
       </c>
       <c r="M2" t="n">
-        <v>0.186569960026257</v>
+        <v>0.208222709856524</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0677260221220837</v>
+        <v>0.10017008984594</v>
       </c>
       <c r="O2" t="n">
-        <v>0.112976565260545</v>
+        <v>0.13959595459099</v>
       </c>
       <c r="P2" t="n">
-        <v>0.045250543138461</v>
+        <v>0.0394258647450503</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.173211589035972</v>
+        <v>0.170638146864122</v>
       </c>
       <c r="R2" t="n">
-        <v>2.84775184101123</v>
+        <v>2.89566232224352</v>
       </c>
       <c r="S2" t="n">
-        <v>0.166033043504158</v>
+        <v>0.159001322731053</v>
       </c>
     </row>
     <row r="3">
@@ -541,58 +538,58 @@
         <v>20</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0927980116674671</v>
+        <v>0.102094121770123</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00317215333648359</v>
+        <v>0.00633447365628936</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00317215333648359</v>
+        <v>0.00633447365628936</v>
       </c>
       <c r="E3" t="n">
-        <v>0.00136335804529152</v>
+        <v>0.00418014764034602</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00256238796535752</v>
+        <v>0.00199638775954267</v>
       </c>
       <c r="G3" t="n">
-        <v>0.00325600217331749</v>
+        <v>0.00118330607935602</v>
       </c>
       <c r="H3" t="n">
-        <v>0.101796407185629</v>
+        <v>0.115</v>
       </c>
       <c r="I3" t="n">
-        <v>0.102740832776952</v>
+        <v>0.114611029530331</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0292855085380335</v>
+        <v>0.0329343323120169</v>
       </c>
       <c r="K3" t="n">
-        <v>0.000857641010331234</v>
+        <v>0.00108467024483836</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0227255475927646</v>
+        <v>0.0150737110775756</v>
       </c>
       <c r="M3" t="n">
-        <v>0.165370974448123</v>
+        <v>0.213173559349694</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0839068350572852</v>
+        <v>0.0931662870527073</v>
       </c>
       <c r="O3" t="n">
-        <v>0.121810978838731</v>
+        <v>0.137895845610196</v>
       </c>
       <c r="P3" t="n">
-        <v>0.0379041437814457</v>
+        <v>0.0447295585574887</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.233698782945591</v>
+        <v>-0.0595052852077916</v>
       </c>
       <c r="R3" t="n">
-        <v>2.86585678048793</v>
+        <v>2.77515888691911</v>
       </c>
       <c r="S3" t="n">
-        <v>0.142645426855359</v>
+        <v>0.198099848272118</v>
       </c>
     </row>
     <row r="4">
@@ -600,58 +597,58 @@
         <v>21</v>
       </c>
       <c r="B4" t="n">
-        <v>0.10599442495418</v>
+        <v>0.0958719165605683</v>
       </c>
       <c r="C4" t="n">
-        <v>0.00385410428541189</v>
+        <v>0.0303518076406184</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00385410428541189</v>
+        <v>0.0303518076406184</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0177534021050044</v>
+        <v>0.00119476880739175</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00205696197348051</v>
+        <v>0.00337695420531697</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0142892774638205</v>
+        <v>0.00378431244310597</v>
       </c>
       <c r="H4" t="n">
-        <v>0.119760479041916</v>
+        <v>0.105</v>
       </c>
       <c r="I4" t="n">
-        <v>0.121906198173184</v>
+        <v>0.1076326177571</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0287972165594354</v>
+        <v>0.037124491469608</v>
       </c>
       <c r="K4" t="n">
-        <v>0.00082927968157102</v>
+        <v>0.00137822786687699</v>
       </c>
       <c r="L4" t="n">
-        <v>0.036734014087846</v>
+        <v>0.00176211874553988</v>
       </c>
       <c r="M4" t="n">
-        <v>0.190784375059278</v>
+        <v>0.200674893666289</v>
       </c>
       <c r="N4" t="n">
-        <v>0.101479058538283</v>
+        <v>0.0795352931145078</v>
       </c>
       <c r="O4" t="n">
-        <v>0.141258121182396</v>
+        <v>0.131079036074453</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0397790626441134</v>
+        <v>0.0515437429599455</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.323896129382166</v>
+        <v>-0.149356350223454</v>
       </c>
       <c r="R4" t="n">
-        <v>2.75133702435462</v>
+        <v>2.56276266577332</v>
       </c>
       <c r="S4" t="n">
-        <v>0.154050360971432</v>
+        <v>0.198912774920749</v>
       </c>
     </row>
     <row r="5">
@@ -659,58 +656,58 @@
         <v>22</v>
       </c>
       <c r="B5" t="n">
-        <v>0.096886197190047</v>
+        <v>0.119788469302521</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0000642518732082847</v>
+        <v>0.00579689808418174</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0000642518732082847</v>
+        <v>0.00579689808418174</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0128365306302788</v>
+        <v>0.0026339623431639</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0046834638715204</v>
+        <v>0.00231796480647126</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00463547120081184</v>
+        <v>0.00397062082672478</v>
       </c>
       <c r="H5" t="n">
-        <v>0.107784431137725</v>
+        <v>0.14</v>
       </c>
       <c r="I5" t="n">
-        <v>0.107438682319503</v>
+        <v>0.139827742172983</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0307874576488748</v>
+        <v>0.0195210508139952</v>
       </c>
       <c r="K5" t="n">
-        <v>0.000947867548481259</v>
+        <v>0.000381071424882581</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0278991340824717</v>
+        <v>0.0761262850892554</v>
       </c>
       <c r="M5" t="n">
-        <v>0.176912489891667</v>
+        <v>0.19910820854102</v>
       </c>
       <c r="N5" t="n">
-        <v>0.0873288937007074</v>
+        <v>0.126264592102627</v>
       </c>
       <c r="O5" t="n">
-        <v>0.129984775477869</v>
+        <v>0.154583573444775</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0426558817771621</v>
+        <v>0.0283189813421478</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.0567826037568824</v>
+        <v>-0.0979871391264475</v>
       </c>
       <c r="R5" t="n">
-        <v>2.54195841927415</v>
+        <v>2.78186157556275</v>
       </c>
       <c r="S5" t="n">
-        <v>0.149013355809195</v>
+        <v>0.122981923451764</v>
       </c>
     </row>
     <row r="6">
@@ -718,117 +715,58 @@
         <v>23</v>
       </c>
       <c r="B6" t="n">
-        <v>0.114185223369407</v>
+        <v>0.0988019168182415</v>
       </c>
       <c r="C6" t="n">
-        <v>0.00434179612031196</v>
+        <v>0.0162065226477038</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00434179612031196</v>
+        <v>0.0162065226477038</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0059451742266941</v>
+        <v>0.00407762982466713</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00518550053203681</v>
+        <v>0.00133574258160425</v>
       </c>
       <c r="G6" t="n">
-        <v>0.00856487138758841</v>
+        <v>0.00168537375991731</v>
       </c>
       <c r="H6" t="n">
-        <v>0.132530120481928</v>
+        <v>0.1075</v>
       </c>
       <c r="I6" t="n">
-        <v>0.132097748401059</v>
+        <v>0.112944066007418</v>
       </c>
       <c r="J6" t="n">
-        <v>0.028085160095287</v>
+        <v>0.0440771493429622</v>
       </c>
       <c r="K6" t="n">
-        <v>0.000788776217577899</v>
+        <v>0.00194279509420179</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0575702556675026</v>
+        <v>-0.0202213956936644</v>
       </c>
       <c r="M6" t="n">
-        <v>0.2022733347902</v>
+        <v>0.225855244061486</v>
       </c>
       <c r="N6" t="n">
-        <v>0.112768413070236</v>
+        <v>0.0788523695502407</v>
       </c>
       <c r="O6" t="n">
-        <v>0.153320567350784</v>
+        <v>0.138009682055858</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0405521542805488</v>
+        <v>0.059157312505617</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.138953225019174</v>
+        <v>-0.29862844077682</v>
       </c>
       <c r="R6" t="n">
-        <v>2.60597754830972</v>
+        <v>2.71264764178681</v>
       </c>
       <c r="S6" t="n">
-        <v>0.144703079122698</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.0964659692295778</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.00864261517229911</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.00864261517229911</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.0096110881873509</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.00983058705122175</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.01740856042971</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.107784431137725</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.105308624192322</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.0308348411695092</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.000950787429948859</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.0332327919407683</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.178622212072324</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.0869784687385928</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.129768889483316</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0.0427904207447236</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0.100116205821406</v>
-      </c>
-      <c r="R7" t="n">
-        <v>2.51503135988293</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0.145389420131556</v>
+        <v>0.24607663975515</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Implementing new execution-engines: batchtools multicore 2. Implementing new execution-engines: batchtools SLURM 3. Implementing new execution-engines: batchtools multicore adaptive 4. Implementing new execution-engines: batchtools SLURM adaptive 5. Implementing new execution-engines: sequential adaptive for param optimization 6. Reworking folder structure for execution engines
</commit_message>
<xml_diff>
--- a/tests/publish_exports/excel_basis_test_singleelement.xlsx
+++ b/tests/publish_exports/excel_basis_test_singleelement.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">split</t>
   </si>
@@ -84,6 +84,27 @@
   </si>
   <si>
     <t xml:space="preserve">split5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">split6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">split7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">split8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">split9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">split10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">split11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">split12</t>
   </si>
 </sst>
 </file>
@@ -479,58 +500,58 @@
         <v>19</v>
       </c>
       <c r="B2" t="n">
-        <v>0.105465445923025</v>
+        <v>0.101372693080076</v>
       </c>
       <c r="C2" t="n">
-        <v>0.00968446487245028</v>
+        <v>0.0193616784843136</v>
       </c>
       <c r="D2" t="n">
-        <v>0.00968446487245028</v>
+        <v>0.0193616784843136</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0101702486418485</v>
+        <v>0.00140909025592797</v>
       </c>
       <c r="F2" t="n">
-        <v>0.00690566616132421</v>
+        <v>0.00164562122528189</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0137561491366818</v>
+        <v>0.00245812981434357</v>
       </c>
       <c r="H2" t="n">
-        <v>0.12</v>
+        <v>0.1125</v>
       </c>
       <c r="I2" t="n">
-        <v>0.117599928568928</v>
+        <v>0.113027303455572</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0284239643932029</v>
+        <v>0.0389091231939749</v>
       </c>
       <c r="K2" t="n">
-        <v>0.000807921751826065</v>
+        <v>0.00151391986772391</v>
       </c>
       <c r="L2" t="n">
-        <v>0.049221387125471</v>
+        <v>0.0176739562047012</v>
       </c>
       <c r="M2" t="n">
-        <v>0.208222709856524</v>
+        <v>0.20850420030241</v>
       </c>
       <c r="N2" t="n">
-        <v>0.10017008984594</v>
+        <v>0.0865213873898316</v>
       </c>
       <c r="O2" t="n">
-        <v>0.13959595459099</v>
+        <v>0.137413768260714</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0394258647450503</v>
+        <v>0.0508923808708829</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.170638146864122</v>
+        <v>0.0234657584626485</v>
       </c>
       <c r="R2" t="n">
-        <v>2.89566232224352</v>
+        <v>2.73746020701035</v>
       </c>
       <c r="S2" t="n">
-        <v>0.159001322731053</v>
+        <v>0.190830244097708</v>
       </c>
     </row>
     <row r="3">
@@ -538,58 +559,58 @@
         <v>20</v>
       </c>
       <c r="B3" t="n">
-        <v>0.102094121770123</v>
+        <v>0.10046021511555</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00633447365628936</v>
+        <v>0.0144790512138432</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00633447365628936</v>
+        <v>0.0144790512138432</v>
       </c>
       <c r="E3" t="n">
-        <v>0.00418014764034602</v>
+        <v>0.018001580428357</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00199638775954267</v>
+        <v>0.00218159093608203</v>
       </c>
       <c r="G3" t="n">
-        <v>0.00118330607935602</v>
+        <v>0.0151366508326402</v>
       </c>
       <c r="H3" t="n">
-        <v>0.115</v>
+        <v>0.1125</v>
       </c>
       <c r="I3" t="n">
-        <v>0.114611029530331</v>
+        <v>0.112604045858018</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0329343323120169</v>
+        <v>0.0313238052198125</v>
       </c>
       <c r="K3" t="n">
-        <v>0.00108467024483836</v>
+        <v>0.000981180773448755</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0150737110775756</v>
+        <v>0.0237092066514161</v>
       </c>
       <c r="M3" t="n">
-        <v>0.213173559349694</v>
+        <v>0.204939171876303</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0931662870527073</v>
+        <v>0.0914140787106087</v>
       </c>
       <c r="O3" t="n">
-        <v>0.137895845610196</v>
+        <v>0.133186093483387</v>
       </c>
       <c r="P3" t="n">
-        <v>0.0447295585574887</v>
+        <v>0.041772014772778</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.0595052852077916</v>
+        <v>0.0350859483886787</v>
       </c>
       <c r="R3" t="n">
-        <v>2.77515888691911</v>
+        <v>2.80552696729519</v>
       </c>
       <c r="S3" t="n">
-        <v>0.198099848272118</v>
+        <v>0.181229965224887</v>
       </c>
     </row>
     <row r="4">
@@ -597,58 +618,58 @@
         <v>21</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0958719165605683</v>
+        <v>0.112591332243283</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0303518076406184</v>
+        <v>0.0379545590941365</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0303518076406184</v>
+        <v>0.0379545590941365</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00119476880739175</v>
+        <v>0.00380383274135115</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00337695420531697</v>
+        <v>0.000718786049232228</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00378431244310597</v>
+        <v>0.00346607303240634</v>
       </c>
       <c r="H4" t="n">
-        <v>0.105</v>
+        <v>0.1275</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1076326177571</v>
+        <v>0.129093582340272</v>
       </c>
       <c r="J4" t="n">
-        <v>0.037124491469608</v>
+        <v>0.0346180264531014</v>
       </c>
       <c r="K4" t="n">
-        <v>0.00137822786687699</v>
+        <v>0.00119840775550763</v>
       </c>
       <c r="L4" t="n">
-        <v>0.00176211874553988</v>
+        <v>0.0299638487524645</v>
       </c>
       <c r="M4" t="n">
-        <v>0.200674893666289</v>
+        <v>0.210824081047105</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0795352931145078</v>
+        <v>0.103167164129265</v>
       </c>
       <c r="O4" t="n">
-        <v>0.131079036074453</v>
+        <v>0.152346525631577</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0515437429599455</v>
+        <v>0.049179361502312</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.149356350223454</v>
+        <v>-0.0296387911169262</v>
       </c>
       <c r="R4" t="n">
-        <v>2.56276266577332</v>
+        <v>2.61297697363255</v>
       </c>
       <c r="S4" t="n">
-        <v>0.198912774920749</v>
+        <v>0.18086023229464</v>
       </c>
     </row>
     <row r="5">
@@ -656,58 +677,58 @@
         <v>22</v>
       </c>
       <c r="B5" t="n">
-        <v>0.119788469302521</v>
+        <v>0.106463720218374</v>
       </c>
       <c r="C5" t="n">
-        <v>0.00579689808418174</v>
+        <v>0.00259086029167145</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00579689808418174</v>
+        <v>0.00259086029167145</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0026339623431639</v>
+        <v>0.0116142837776102</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00231796480647126</v>
+        <v>0.00689921471761576</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00397062082672478</v>
+        <v>0.0146199848028807</v>
       </c>
       <c r="H5" t="n">
-        <v>0.14</v>
+        <v>0.12</v>
       </c>
       <c r="I5" t="n">
-        <v>0.139827742172983</v>
+        <v>0.120795152169705</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0195210508139952</v>
+        <v>0.0371723622659704</v>
       </c>
       <c r="K5" t="n">
-        <v>0.000381071424882581</v>
+        <v>0.00138178451643254</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0761262850892554</v>
+        <v>0.0122968202531281</v>
       </c>
       <c r="M5" t="n">
-        <v>0.19910820854102</v>
+        <v>0.2184579569549</v>
       </c>
       <c r="N5" t="n">
-        <v>0.126264592102627</v>
+        <v>0.0935984236687816</v>
       </c>
       <c r="O5" t="n">
-        <v>0.154583573444775</v>
+        <v>0.145313583992451</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0283189813421478</v>
+        <v>0.0517151603236695</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.0979871391264475</v>
+        <v>-0.0756449778676953</v>
       </c>
       <c r="R5" t="n">
-        <v>2.78186157556275</v>
+        <v>2.78817320719854</v>
       </c>
       <c r="S5" t="n">
-        <v>0.122981923451764</v>
+        <v>0.206161136701772</v>
       </c>
     </row>
     <row r="6">
@@ -715,58 +736,471 @@
         <v>23</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0988019168182415</v>
+        <v>0.0889259959103077</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0162065226477038</v>
+        <v>0.0220076562015574</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0162065226477038</v>
+        <v>0.0220076562015574</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00407762982466713</v>
+        <v>0.0187369856422</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00133574258160425</v>
+        <v>0.00901537533494128</v>
       </c>
       <c r="G6" t="n">
-        <v>0.00168537375991731</v>
+        <v>0.0217258177888834</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1075</v>
+        <v>0.095</v>
       </c>
       <c r="I6" t="n">
-        <v>0.112944066007418</v>
+        <v>0.0946501159758657</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0440771493429622</v>
+        <v>0.0459948848454132</v>
       </c>
       <c r="K6" t="n">
-        <v>0.00194279509420179</v>
+        <v>0.00211552943194282</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.0202213956936644</v>
+        <v>-0.0278752640308697</v>
       </c>
       <c r="M6" t="n">
-        <v>0.225855244061486</v>
+        <v>0.223652274281097</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0788523695502407</v>
+        <v>0.0645301206913722</v>
       </c>
       <c r="O6" t="n">
-        <v>0.138009682055858</v>
+        <v>0.128660445321065</v>
       </c>
       <c r="P6" t="n">
-        <v>0.059157312505617</v>
+        <v>0.0641303246296926</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.29862844077682</v>
+        <v>-0.0524809465261223</v>
       </c>
       <c r="R6" t="n">
-        <v>2.71264764178681</v>
+        <v>2.71805941182002</v>
       </c>
       <c r="S6" t="n">
-        <v>0.24607663975515</v>
+        <v>0.251527538311966</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.0883233011276117</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0445648683056284</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0445648683056284</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.017932973743282</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.00378486561380995</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0172317260901666</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.0967711986361649</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.0436241438185123</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.00190306592389824</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-0.027693448305193</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.212247095049935</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.0626516684094374</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.125982980578076</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.0633313121686391</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-0.0571276396796375</v>
+      </c>
+      <c r="R7" t="n">
+        <v>2.48077914718214</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.239940543355128</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.102242203522032</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0104117573034624</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0104117573034624</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0162009553905668</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.00349439646177226</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0145164934189382</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.115</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.113419326473793</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.0279821969096232</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.000783003343888928</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.0266394892242237</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.185782273444934</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.0964566659428646</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.134629654362288</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.0381729884194233</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-0.111761065816862</v>
+      </c>
+      <c r="R8" t="n">
+        <v>2.80135773723407</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.15914278422071</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.101992498841151</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.00708088700961443</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.00708088700961443</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.0139512146274052</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.00242301575106764</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0123631828830953</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.115</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.115511576241257</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.0322577931069022</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.00104056521612771</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.0221682548221736</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.225839728147332</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.0912679245178811</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.138494915079587</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.0472269905617058</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-0.0428874865245892</v>
+      </c>
+      <c r="R9" t="n">
+        <v>2.74594939913908</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.203671473325159</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.11124205563887</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.00849745896614226</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.00849745896614226</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0236910370333491</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.00610480407794362</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0226632723149329</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.1275</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.128168230754276</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.0224841626008159</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.000505537567859929</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.0669171013497296</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.201842738511121</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.111928950113827</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.14271326663124</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.0307843165174128</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.00752765833299014</v>
+      </c>
+      <c r="R10" t="n">
+        <v>2.79754978461519</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.134925637161391</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.112980849764866</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0133521605026819</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0133521605026819</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.00586152307595394</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0016075822668267</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.00279793542104498</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.127711211838299</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.0296298867840741</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.000877930190837048</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.0549643700783292</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.20987075765165</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.108079583302763</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.150831400616283</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.0427518173135197</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.0776323876819894</v>
+      </c>
+      <c r="R11" t="n">
+        <v>2.71169724423418</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.154906387573321</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.0922710699988148</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0161708231722629</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0161708231722629</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0229680639011116</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.00359211093131291</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0189856251557126</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.100331892724322</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.0380923633475028</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.00145102814539818</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.00882858375323894</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.22541852203775</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.0747877291157078</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.123196575615165</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.0484088464994573</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.190379901319416</v>
+      </c>
+      <c r="R12" t="n">
+        <v>2.96824149860433</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.216589938284511</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.0936152742390237</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0348265335563007</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0348265335563007</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.00176252665917453</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.00060264078786279</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.00171316344279474</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.1025</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.103511448859905</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.0428198297223629</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.00183353781745215</v>
+      </c>
+      <c r="L13" t="n">
+        <v>-0.0197383722339294</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.218407803229745</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.0734210946574579</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.131648962107737</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.0582278674502794</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>-0.190493197634822</v>
+      </c>
+      <c r="R13" t="n">
+        <v>2.77065510915612</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.238146175463674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removing the fairness-footprint from the framework to make it open to a wider use-case. Fairness is still a perfect fit in use, but other processing-reasons are possible as well.
</commit_message>
<xml_diff>
--- a/tests/publish_exports/excel_basis_test_singleelement.xlsx
+++ b/tests/publish_exports/excel_basis_test_singleelement.xlsx
@@ -467,7 +467,7 @@
         <v>19</v>
       </c>
       <c r="B2" t="n">
-        <v>0.104997005519039</v>
+        <v>0.10561669283312</v>
       </c>
       <c r="C2" t="n">
         <v>0.0346943664819284</v>
@@ -482,13 +482,13 @@
         <v>0.00249326069621592</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00506455245660281</v>
+        <v>0.00506455245660282</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1175</v>
+        <v>0.0926064804802312</v>
       </c>
       <c r="I2" t="n">
-        <v>0.11701981837233</v>
+        <v>0.0921262988525608</v>
       </c>
       <c r="J2" t="n">
         <v>0.0191367936453366</v>
@@ -497,22 +497,22 @@
         <v>0.000366216871024195</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0804046734415772</v>
+        <v>0.0555111539218084</v>
       </c>
       <c r="M2" t="n">
-        <v>0.160047036285309</v>
+        <v>0.13515351676554</v>
       </c>
       <c r="N2" t="n">
-        <v>0.098725685453533</v>
+        <v>0.0738321659337642</v>
       </c>
       <c r="O2" t="n">
-        <v>0.134783355692578</v>
+        <v>0.109889836172809</v>
       </c>
       <c r="P2" t="n">
         <v>0.0360576702390452</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.00321310532969555</v>
+        <v>0.00321310532969494</v>
       </c>
       <c r="R2" t="n">
         <v>1.62120504076009</v>

</xml_diff>